<commit_message>
[mod] ImportStructure [add] ExcelWorkBook.getSheetXXX Optional<ExcelSheet> 로 수정
</commit_message>
<xml_diff>
--- a/src/test/resources/tutorial/excluded-Header-Multi-Student.xlsx
+++ b/src/test/resources/tutorial/excluded-Header-Multi-Student.xlsx
@@ -60,14 +60,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -87,26 +81,26 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="5">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="8">
+      <c r="B1" t="s" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="6">
+      <c r="A2" t="s" s="3">
         <v>2</v>
       </c>
-      <c r="B2" t="n" s="9">
+      <c r="B2" t="n" s="6">
         <v>20.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="6">
+      <c r="A3" t="s" s="3">
         <v>3</v>
       </c>
-      <c r="B3" t="n" s="9">
+      <c r="B3" t="n" s="6">
         <v>23.0</v>
       </c>
     </row>

</xml_diff>